<commit_message>
reducing demand on RAM by: downcasting bytes, only buffering when truly necessary, and deleting datasets once they are done being used
</commit_message>
<xml_diff>
--- a/cableSettings.xlsx
+++ b/cableSettings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ers334\Documents\gitRepos\preprocess_DAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:2001_{86AFD6D5-7E75-4745-BF72-715D947330CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49EDB104-6F18-41F1-B7A5-EB60C106BC30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C7A9485E-BE60-49EE-BF9E-665F504FA5B3}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="cableSettings" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>Dataset</t>
   </si>
@@ -72,30 +71,12 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Worth splitting into two?</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>Worth splitting into three?</t>
-  </si>
-  <si>
     <t>start_distance_km[0]</t>
   </si>
   <si>
-    <t>start_distance_km[1]</t>
-  </si>
-  <si>
-    <t>start_distance_km[2]</t>
-  </si>
-  <si>
     <t>OOI_Silixa_South</t>
   </si>
   <si>
-    <t>Probably the same as above</t>
-  </si>
-  <si>
     <t>interrogator</t>
   </si>
   <si>
@@ -111,14 +92,32 @@
     <t>Svalbard</t>
   </si>
   <si>
-    <t>What segments to use?</t>
+    <t>data_dimensions</t>
+  </si>
+  <si>
+    <t>Memory_GB</t>
+  </si>
+  <si>
+    <t>file_durations_sec</t>
+  </si>
+  <si>
+    <t>Too big, can't use full cable</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>cable_length_km</t>
+  </si>
+  <si>
+    <t>full</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,6 +263,11 @@
       <color theme="1"/>
       <name val="Aptos Display"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="33">
@@ -607,10 +611,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -986,28 +993,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5E93172-BDC0-4D7D-9EA8-0BCC176EBE0A}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.7109375" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -1016,36 +1027,43 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="L1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1">
         <v>72.727272727272705</v>
@@ -1053,36 +1071,46 @@
       <c r="D2" s="2">
         <v>727</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="2">
+        <f>D2/C2</f>
+        <v>9.9962500000000034</v>
+      </c>
+      <c r="F2" s="1">
         <v>4.0807521676988996</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>13000</v>
       </c>
-      <c r="G2" s="2">
+      <c r="H2" s="2">
+        <f>G2*D2</f>
+        <v>9451000</v>
+      </c>
+      <c r="I2" s="2">
+        <f>(64/8)*H2/(2^30)</f>
+        <v>7.04154372215271E-2</v>
+      </c>
+      <c r="J2" s="2">
         <v>1.02</v>
       </c>
-      <c r="H2" s="2">
-        <f t="shared" ref="H2:H7" si="0">F2*E2</f>
+      <c r="K2" s="2">
+        <f>G2*F2</f>
         <v>53049.778180085697</v>
       </c>
-      <c r="I2" s="2">
-        <v>-40.01</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" s="2"/>
+      <c r="L2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2">
         <v>500</v>
@@ -1091,37 +1119,45 @@
         <v>15000</v>
       </c>
       <c r="E3" s="2">
+        <f t="shared" ref="E3:E7" si="0">D3/C3</f>
+        <v>30</v>
+      </c>
+      <c r="F3" s="2">
         <v>2.0419046999999999</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <v>32600</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
+        <f>G3*D3</f>
+        <v>489000000</v>
+      </c>
+      <c r="I3" s="2">
+        <f t="shared" ref="I3:I7" si="1">(64/8)*H3/(2^30)</f>
+        <v>3.643333911895752</v>
+      </c>
+      <c r="J3" s="2">
         <v>30.628571999999998</v>
       </c>
-      <c r="H3" s="2">
-        <f t="shared" si="0"/>
+      <c r="K3" s="2">
+        <f>G3*F3</f>
         <v>66566.093219999995</v>
       </c>
-      <c r="I3" s="2">
-        <v>-40.01</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="L3" s="2">
+        <v>20</v>
+      </c>
+      <c r="M3" s="2">
+        <f>K3/1000-L3</f>
+        <v>46.566093219999999</v>
+      </c>
+      <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2">
         <v>1000</v>
@@ -1130,37 +1166,48 @@
         <v>30000</v>
       </c>
       <c r="E4" s="2">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="F4" s="2">
         <v>2.0419046999999999</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4" s="2">
         <v>32600</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
+        <f>G4*D4</f>
+        <v>978000000</v>
+      </c>
+      <c r="I4" s="2">
+        <f t="shared" si="1"/>
+        <v>7.2866678237915039</v>
+      </c>
+      <c r="J4" s="2">
         <v>30.628571999999998</v>
       </c>
-      <c r="H4" s="2">
-        <f t="shared" si="0"/>
+      <c r="K4" s="2">
+        <f>G4*F4</f>
         <v>66566.093219999995</v>
       </c>
-      <c r="I4" s="2">
-        <v>-40.01</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>12</v>
+      <c r="L4" s="2">
+        <v>20</v>
+      </c>
+      <c r="M4" s="2">
+        <f>K4/1000-L4</f>
+        <v>46.566093219999999</v>
+      </c>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2">
         <v>200</v>
@@ -1169,37 +1216,48 @@
         <v>12000</v>
       </c>
       <c r="E5" s="2">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="F5" s="2">
         <v>2.0419046999999999</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
         <v>47500</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
+        <f>G5*D5</f>
+        <v>570000000</v>
+      </c>
+      <c r="I5" s="2">
+        <f t="shared" si="1"/>
+        <v>4.246830940246582</v>
+      </c>
+      <c r="J5" s="2">
         <v>51.047620000000002</v>
       </c>
-      <c r="H5" s="2">
-        <f t="shared" si="0"/>
+      <c r="K5" s="2">
+        <f>G5*F5</f>
         <v>96990.473249999995</v>
       </c>
-      <c r="I5" s="2">
-        <v>-40.01</v>
-      </c>
-      <c r="J5" s="2">
-        <v>-80.010000000000005</v>
-      </c>
-      <c r="K5" s="2" t="s">
+      <c r="L5" s="2">
+        <v>20</v>
+      </c>
+      <c r="M5" s="2">
+        <f>K5/1000-L5</f>
+        <v>76.990473249999994</v>
+      </c>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L5" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2">
         <v>1000</v>
@@ -1208,31 +1266,43 @@
         <v>15000</v>
       </c>
       <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F6" s="2">
         <v>1</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G6" s="2">
         <v>19648</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
+        <f>G6*D6</f>
+        <v>294720000</v>
+      </c>
+      <c r="I6" s="2">
+        <f t="shared" si="1"/>
+        <v>2.1958351135253906</v>
+      </c>
+      <c r="J6" s="2">
         <v>2.0419047677428099</v>
       </c>
-      <c r="H6" s="2">
-        <f t="shared" si="0"/>
+      <c r="K6" s="2">
+        <f>G6*F6</f>
         <v>19648</v>
       </c>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
       <c r="L6" s="2" t="s">
-        <v>19</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15">
       <c r="A7" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C7" s="2">
         <v>625</v>
@@ -1241,30 +1311,48 @@
         <v>6250</v>
       </c>
       <c r="E7" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F7" s="2">
         <v>4.0852007630987197</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G7" s="1">
         <v>33748</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="2">
+        <f>G7*D7</f>
+        <v>210925000</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" si="1"/>
+        <v>1.5715137124061584</v>
+      </c>
+      <c r="J7" s="1">
         <v>8.1704015261974501</v>
       </c>
-      <c r="H7" s="2">
-        <f t="shared" si="0"/>
+      <c r="K7" s="2">
+        <f>G7*F7</f>
         <v>137867.35535305558</v>
       </c>
-      <c r="I7" s="2">
-        <v>-40.01</v>
-      </c>
-      <c r="J7" s="2">
-        <v>-80.010000000000005</v>
-      </c>
-      <c r="K7" s="2">
-        <v>-120.01</v>
-      </c>
       <c r="L7" s="2" t="s">
-        <v>25</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="G14">
+        <f>7.3/19.3</f>
+        <v>0.37823834196891187</v>
+      </c>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix timestamp error in data files
</commit_message>
<xml_diff>
--- a/cableSettings.xlsx
+++ b/cableSettings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ers334\Documents\gitRepos\preprocess_DAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49EDB104-6F18-41F1-B7A5-EB60C106BC30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77553ED5-F1F7-471E-A1D3-45DC4BD7549B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C7A9485E-BE60-49EE-BF9E-665F504FA5B3}"/>
+    <workbookView xWindow="22932" yWindow="732" windowWidth="23256" windowHeight="13896" xr2:uid="{C7A9485E-BE60-49EE-BF9E-665F504FA5B3}"/>
   </bookViews>
   <sheets>
     <sheet name="cableSettings" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>Dataset</t>
   </si>
@@ -104,13 +104,13 @@
     <t>Too big, can't use full cable</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>cable_length_km</t>
   </si>
   <si>
-    <t>full</t>
+    <t>new_data_dimension</t>
+  </si>
+  <si>
+    <t>new_memory_GB</t>
   </si>
 </sst>
 </file>
@@ -993,10 +993,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5E93172-BDC0-4D7D-9EA8-0BCC176EBE0A}">
-  <dimension ref="A1:O16"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1010,10 +1010,10 @@
     <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="19.42578125" customWidth="1"/>
+    <col min="13" max="15" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1051,14 +1051,19 @@
         <v>12</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="2"/>
       <c r="O1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:16">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1096,16 +1101,24 @@
         <f>G2*F2</f>
         <v>53049.778180085697</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
+      <c r="L2" s="2">
+        <v>0</v>
+      </c>
+      <c r="M2" s="2">
+        <f>K2/1000-L2</f>
+        <v>53.049778180085696</v>
+      </c>
+      <c r="N2" s="2">
+        <f t="shared" ref="N2:N7" si="0">ROUND(1000*M2/F2, 0)*D2</f>
+        <v>9451000</v>
+      </c>
+      <c r="O2" s="2">
+        <f t="shared" ref="O2:O3" si="1">(32/8)*N2/(2^30)</f>
+        <v>3.520771861076355E-2</v>
+      </c>
+      <c r="P2" s="2"/>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:16">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -1119,7 +1132,7 @@
         <v>15000</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E7" si="0">D3/C3</f>
+        <f t="shared" ref="E3:E7" si="2">D3/C3</f>
         <v>30</v>
       </c>
       <c r="F3" s="2">
@@ -1133,7 +1146,7 @@
         <v>489000000</v>
       </c>
       <c r="I3" s="2">
-        <f t="shared" ref="I3:I7" si="1">(64/8)*H3/(2^30)</f>
+        <f t="shared" ref="I3:I7" si="3">(64/8)*H3/(2^30)</f>
         <v>3.643333911895752</v>
       </c>
       <c r="J3" s="2">
@@ -1150,9 +1163,16 @@
         <f>K3/1000-L3</f>
         <v>46.566093219999999</v>
       </c>
-      <c r="N3" s="2"/>
+      <c r="N3" s="2">
+        <f>ROUND(1000*M3/F3, 0)*D3</f>
+        <v>342075000</v>
+      </c>
+      <c r="O3" s="2">
+        <f t="shared" si="1"/>
+        <v>1.2743286788463593</v>
+      </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:16">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -1166,7 +1186,7 @@
         <v>30000</v>
       </c>
       <c r="E4" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="F4" s="2">
@@ -1180,7 +1200,7 @@
         <v>978000000</v>
       </c>
       <c r="I4" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.2866678237915039</v>
       </c>
       <c r="J4" s="2">
@@ -1197,12 +1217,19 @@
         <f>K4/1000-L4</f>
         <v>46.566093219999999</v>
       </c>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2" t="s">
+      <c r="N4" s="2">
+        <f t="shared" si="0"/>
+        <v>684150000</v>
+      </c>
+      <c r="O4" s="2">
+        <f>(32/8)*N4/(2^30)</f>
+        <v>2.5486573576927185</v>
+      </c>
+      <c r="P4" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:16">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1216,7 +1243,7 @@
         <v>12000</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="F5" s="2">
@@ -1230,7 +1257,7 @@
         <v>570000000</v>
       </c>
       <c r="I5" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.246830940246582</v>
       </c>
       <c r="J5" s="2">
@@ -1247,12 +1274,19 @@
         <f>K5/1000-L5</f>
         <v>76.990473249999994</v>
       </c>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2" t="s">
+      <c r="N5" s="2">
+        <f t="shared" si="0"/>
+        <v>452460000</v>
+      </c>
+      <c r="O5" s="2">
+        <f t="shared" ref="O5:O7" si="4">(32/8)*N5/(2^30)</f>
+        <v>1.6855448484420776</v>
+      </c>
+      <c r="P5" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -1266,7 +1300,7 @@
         <v>15000</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="F6" s="2">
@@ -1280,7 +1314,7 @@
         <v>294720000</v>
       </c>
       <c r="I6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.1958351135253906</v>
       </c>
       <c r="J6" s="2">
@@ -1290,14 +1324,24 @@
         <f>G6*F6</f>
         <v>19648</v>
       </c>
-      <c r="L6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
+      <c r="L6" s="2">
+        <v>0</v>
+      </c>
+      <c r="M6" s="2">
+        <f t="shared" ref="M6:M7" si="5">K6/1000-L6</f>
+        <v>19.648</v>
+      </c>
+      <c r="N6" s="2">
+        <f t="shared" si="0"/>
+        <v>294720000</v>
+      </c>
+      <c r="O6" s="2">
+        <f t="shared" si="4"/>
+        <v>1.0979175567626953</v>
+      </c>
+      <c r="P6" s="2"/>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:16">
       <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
@@ -1311,7 +1355,7 @@
         <v>6250</v>
       </c>
       <c r="E7" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="F7" s="2">
@@ -1325,7 +1369,7 @@
         <v>210925000</v>
       </c>
       <c r="I7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.5715137124061584</v>
       </c>
       <c r="J7" s="1">
@@ -1335,22 +1379,27 @@
         <f>G7*F7</f>
         <v>137867.35535305558</v>
       </c>
-      <c r="L7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
+      <c r="L7" s="2">
+        <v>40</v>
+      </c>
+      <c r="M7" s="2">
+        <v>100</v>
+      </c>
+      <c r="N7" s="2">
+        <f t="shared" si="0"/>
+        <v>152993750</v>
+      </c>
+      <c r="O7" s="2">
+        <f t="shared" si="4"/>
+        <v>0.56994613260030746</v>
+      </c>
+      <c r="P7" s="2"/>
     </row>
-    <row r="14" spans="1:15">
-      <c r="G14">
-        <f>7.3/19.3</f>
-        <v>0.37823834196891187</v>
-      </c>
+    <row r="14" spans="1:16">
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:16">
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>

</xml_diff>